<commit_message>
Added temperature to the pH measurements
</commit_message>
<xml_diff>
--- a/wk22_pH.xlsx
+++ b/wk22_pH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwdec\Documents\pH-Conversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E450778C-B767-4487-B84C-F7D0E9B9AC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1819F67-F627-4FFE-9BEE-28AE91E2B916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="0" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="200">
   <si>
     <t>Sample identification number</t>
   </si>
@@ -633,13 +633,20 @@
   <si>
     <t>pH_f</t>
   </si>
+  <si>
+    <t>temp_c</t>
+  </si>
+  <si>
+    <t>15,7</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -695,7 +702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -717,6 +724,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -50266,10 +50276,10 @@
   <dimension ref="A1:O149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B130" sqref="A130:B132"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50287,6 +50297,9 @@
       <c r="B1" s="5" t="s">
         <v>197</v>
       </c>
+      <c r="C1" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -50306,6 +50319,9 @@
       <c r="B2" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -50314,6 +50330,9 @@
       <c r="B3" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C3" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -50322,6 +50341,9 @@
       <c r="B4" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C4" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -50330,6 +50352,9 @@
       <c r="B5" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C5" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -50338,6 +50363,9 @@
       <c r="B6" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C6" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -50346,6 +50374,9 @@
       <c r="B7" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C7" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -50354,6 +50385,9 @@
       <c r="B8" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C8" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -50362,6 +50396,9 @@
       <c r="B9" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C9" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -50370,6 +50407,9 @@
       <c r="B10" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C10" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -50378,6 +50418,9 @@
       <c r="B11" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C11" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -50386,6 +50429,9 @@
       <c r="B12" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C12" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -50394,6 +50440,9 @@
       <c r="B13" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C13" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -50402,6 +50451,9 @@
       <c r="B14" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C14" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -50410,6 +50462,9 @@
       <c r="B15" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C15" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -50418,517 +50473,713 @@
       <c r="B16" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>51</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>59</v>
       </c>
       <c r="B19" s="5">
         <v>7.81</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="9">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>60</v>
       </c>
       <c r="B20" s="5">
         <v>7.88</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="9">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B21" s="5">
         <v>7.77</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="9">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>62</v>
       </c>
       <c r="B22" s="5">
         <v>7.93</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="9">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>63</v>
       </c>
       <c r="B23" s="5">
         <v>7.94</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="9">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B24" s="5">
         <v>7.72</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="9">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>65</v>
       </c>
       <c r="B25" s="5">
         <v>7.84</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="9">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>66</v>
       </c>
       <c r="B26" s="5">
         <v>7.8</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="9">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>67</v>
       </c>
       <c r="B27" s="5">
         <v>7.89</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" s="9">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>68</v>
       </c>
       <c r="B28" s="5">
         <v>7.81</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="9">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B29" s="5">
         <v>7.87</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="9">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B30" s="5">
         <v>7.88</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="9">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="5">
         <v>7.87</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="9">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B32" s="5">
         <v>7.87</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="5">
-        <v>7.83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="5">
-        <v>7.82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="5">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="5">
-        <v>7.78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B37" s="5">
-        <v>7.75</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B38" s="5">
-        <v>7.69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>83</v>
       </c>
       <c r="B39" s="5">
         <v>7.77</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" s="9">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B40" s="5">
         <v>7.78</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" s="9">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B41" s="5">
         <v>7.85</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" s="9">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B42" s="5">
         <v>7.97</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" s="9">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>87</v>
       </c>
       <c r="B43" s="5">
         <v>7.78</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" s="9">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B44" s="5">
         <v>7.81</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" s="9">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>89</v>
       </c>
       <c r="B45" s="5">
         <v>7.87</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" s="9">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>90</v>
       </c>
       <c r="B46" s="5">
         <v>7.88</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" s="9">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B47" s="5">
         <v>7.93</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" s="9">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>92</v>
       </c>
       <c r="B48" s="5">
         <v>7.85</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" s="9">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B49" s="5">
         <v>7.88</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" s="9">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>94</v>
       </c>
       <c r="B50" s="5">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B51" s="5">
         <v>7.85</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" s="9">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>98</v>
       </c>
       <c r="B52" s="5">
         <v>7.81</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>99</v>
       </c>
       <c r="B53" s="5">
         <v>7.79</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" s="9">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>100</v>
       </c>
       <c r="B54" s="5">
         <v>7.78</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" s="9">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B55" s="5">
         <v>7.74</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" s="9">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B56" s="5">
         <v>7.81</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" s="9">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>103</v>
       </c>
       <c r="B57" s="5">
         <v>7.74</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" s="9">
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B58" s="5">
         <v>7.85</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B59" s="5">
         <v>7.83</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" s="9">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B60" s="5">
         <v>7.83</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B61" s="5">
         <v>7.83</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" s="9">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B62" s="5">
         <v>7.84</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" s="9">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B63" s="5">
         <v>7.8</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" s="9">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B64" s="5">
         <v>7.72</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64" s="9">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B65" s="5">
         <v>7.81</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" s="9">
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B66" s="5">
         <v>7.83</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66" s="9">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B67" s="5">
         <v>7.84</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" s="9">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B68" s="5">
         <v>7.85</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" s="9">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>115</v>
       </c>
       <c r="B69" s="5">
         <v>7.83</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69" s="9">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>116</v>
       </c>
       <c r="B70" s="5">
         <v>7.83</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70" s="9">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>117</v>
       </c>
       <c r="B71" s="5">
         <v>7.83</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" s="9">
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>118</v>
       </c>
       <c r="B72" s="5">
         <v>7.15</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72" s="9">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>119</v>
       </c>
       <c r="B73" s="5">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73" s="9">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>120</v>
       </c>
       <c r="B74" s="5">
         <v>7.88</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74" s="9">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B75" s="5">
         <v>7.86</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="9">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B76" s="5">
         <v>7.85</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76" s="9">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B77" s="5">
         <v>7.82</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77" s="9">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B78" s="5">
         <v>7.93</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78" s="9">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B79" s="5">
         <v>7.96</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79" s="9">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B80" s="5">
         <v>7.95</v>
+      </c>
+      <c r="C80" s="9">
+        <v>15.2</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -50938,6 +51189,9 @@
       <c r="B81" s="5">
         <v>7.94</v>
       </c>
+      <c r="C81" s="9">
+        <v>15.3</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
@@ -50946,6 +51200,9 @@
       <c r="B82" s="5">
         <v>7.89</v>
       </c>
+      <c r="C82" s="9">
+        <v>15.5</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
@@ -50954,6 +51211,9 @@
       <c r="B83" s="5">
         <v>7.92</v>
       </c>
+      <c r="C83" s="9">
+        <v>15.8</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
@@ -50962,6 +51222,9 @@
       <c r="B84" s="5">
         <v>7.91</v>
       </c>
+      <c r="C84" s="9">
+        <v>15.1</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
@@ -50970,6 +51233,9 @@
       <c r="B85" s="5">
         <v>7.94</v>
       </c>
+      <c r="C85" s="9">
+        <v>14.1</v>
+      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
@@ -50978,6 +51244,9 @@
       <c r="B86" s="5">
         <v>7.91</v>
       </c>
+      <c r="C86" s="9">
+        <v>14.7</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
@@ -50986,6 +51255,9 @@
       <c r="B87" s="5">
         <v>7.93</v>
       </c>
+      <c r="C87" s="9">
+        <v>14.9</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
@@ -50994,6 +51266,9 @@
       <c r="B88" s="5">
         <v>7.91</v>
       </c>
+      <c r="C88" s="9">
+        <v>14.8</v>
+      </c>
       <c r="D88"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -51003,6 +51278,9 @@
       <c r="B89" s="5">
         <v>7.94</v>
       </c>
+      <c r="C89" s="9">
+        <v>15</v>
+      </c>
       <c r="D89"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -51012,6 +51290,9 @@
       <c r="B90" s="5">
         <v>7.81</v>
       </c>
+      <c r="C90" s="9">
+        <v>16.600000000000001</v>
+      </c>
       <c r="D90"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -51021,6 +51302,9 @@
       <c r="B91" s="5">
         <v>7.68</v>
       </c>
+      <c r="C91" s="9">
+        <v>18.7</v>
+      </c>
       <c r="D91"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -51030,6 +51314,9 @@
       <c r="B92" s="5">
         <v>7.81</v>
       </c>
+      <c r="C92" s="9">
+        <v>17.399999999999999</v>
+      </c>
       <c r="D92"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -51039,6 +51326,9 @@
       <c r="B93" s="5">
         <v>7.84</v>
       </c>
+      <c r="C93" s="9">
+        <v>16.7</v>
+      </c>
       <c r="D93"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -51048,6 +51338,9 @@
       <c r="B94" s="5">
         <v>7.94</v>
       </c>
+      <c r="C94" s="9">
+        <v>15.3</v>
+      </c>
       <c r="D94"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -51057,6 +51350,9 @@
       <c r="B95" s="5">
         <v>7.83</v>
       </c>
+      <c r="C95" s="9">
+        <v>16.399999999999999</v>
+      </c>
       <c r="D95"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -51066,6 +51362,9 @@
       <c r="B96" s="5">
         <v>7.82</v>
       </c>
+      <c r="C96" s="9">
+        <v>17.899999999999999</v>
+      </c>
       <c r="D96"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -51075,6 +51374,9 @@
       <c r="B97" s="5">
         <v>8.01</v>
       </c>
+      <c r="C97" s="9">
+        <v>18</v>
+      </c>
       <c r="D97"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -51084,6 +51386,9 @@
       <c r="B98" s="5">
         <v>7.8</v>
       </c>
+      <c r="C98" s="9">
+        <v>18.100000000000001</v>
+      </c>
       <c r="D98"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -51093,6 +51398,9 @@
       <c r="B99" s="5">
         <v>7.85</v>
       </c>
+      <c r="C99" s="9">
+        <v>20.8</v>
+      </c>
       <c r="D99"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -51102,6 +51410,9 @@
       <c r="B100" s="5">
         <v>7.86</v>
       </c>
+      <c r="C100" s="9">
+        <v>20.399999999999999</v>
+      </c>
       <c r="D100"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -51111,6 +51422,9 @@
       <c r="B101" s="5">
         <v>7.86</v>
       </c>
+      <c r="C101" s="9">
+        <v>18.5</v>
+      </c>
       <c r="D101"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -51120,6 +51434,9 @@
       <c r="B102" s="5">
         <v>7.92</v>
       </c>
+      <c r="C102" s="9" t="s">
+        <v>199</v>
+      </c>
       <c r="D102"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -51129,6 +51446,9 @@
       <c r="B103" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C103" s="9" t="s">
+        <v>196</v>
+      </c>
       <c r="D103"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -51138,6 +51458,9 @@
       <c r="B104" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C104" s="9" t="s">
+        <v>196</v>
+      </c>
       <c r="D104"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -51147,6 +51470,9 @@
       <c r="B105" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C105" s="9" t="s">
+        <v>196</v>
+      </c>
       <c r="D105"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -51156,6 +51482,9 @@
       <c r="B106" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C106" s="9" t="s">
+        <v>196</v>
+      </c>
       <c r="D106"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -51165,6 +51494,9 @@
       <c r="B107" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C107" s="9" t="s">
+        <v>196</v>
+      </c>
       <c r="D107"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -51174,6 +51506,9 @@
       <c r="B108" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C108" s="9" t="s">
+        <v>196</v>
+      </c>
       <c r="D108"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -51183,6 +51518,9 @@
       <c r="B109" s="5" t="s">
         <v>196</v>
       </c>
+      <c r="C109" s="9" t="s">
+        <v>196</v>
+      </c>
       <c r="D109"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -51192,6 +51530,9 @@
       <c r="B110" s="5">
         <v>7.85</v>
       </c>
+      <c r="C110" s="9">
+        <v>18.899999999999999</v>
+      </c>
       <c r="D110"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -51201,6 +51542,9 @@
       <c r="B111" s="5">
         <v>7.81</v>
       </c>
+      <c r="C111" s="9">
+        <v>18.7</v>
+      </c>
       <c r="D111"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -51210,6 +51554,9 @@
       <c r="B112" s="5">
         <v>7.83</v>
       </c>
+      <c r="C112" s="9">
+        <v>19.100000000000001</v>
+      </c>
       <c r="D112"/>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
@@ -51219,6 +51566,9 @@
       <c r="B113" s="5">
         <v>7.85</v>
       </c>
+      <c r="C113" s="9">
+        <v>19.2</v>
+      </c>
       <c r="D113"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
@@ -51228,6 +51578,9 @@
       <c r="B114" s="5">
         <v>8.0500000000000007</v>
       </c>
+      <c r="C114" s="9">
+        <v>19.100000000000001</v>
+      </c>
       <c r="D114"/>
       <c r="O114" s="3"/>
     </row>
@@ -51238,6 +51591,9 @@
       <c r="B115" s="5">
         <v>8.0500000000000007</v>
       </c>
+      <c r="C115" s="9">
+        <v>19</v>
+      </c>
       <c r="D115"/>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
@@ -51247,6 +51603,9 @@
       <c r="B116" s="5">
         <v>7.85</v>
       </c>
+      <c r="C116" s="9">
+        <v>18.8</v>
+      </c>
       <c r="D116"/>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
@@ -51256,6 +51615,9 @@
       <c r="B117" s="5">
         <v>7.92</v>
       </c>
+      <c r="C117" s="9">
+        <v>18.899999999999999</v>
+      </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
@@ -51264,6 +51626,9 @@
       <c r="B118" s="5">
         <v>7.76</v>
       </c>
+      <c r="C118" s="9">
+        <v>15.3</v>
+      </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
@@ -51272,6 +51637,7 @@
       <c r="B119" s="5">
         <v>7.81</v>
       </c>
+      <c r="C119" s="9"/>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
@@ -51280,6 +51646,9 @@
       <c r="B120" s="5">
         <v>7.82</v>
       </c>
+      <c r="C120" s="9">
+        <v>15.2</v>
+      </c>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
@@ -51288,6 +51657,9 @@
       <c r="B121" s="5">
         <v>7.89</v>
       </c>
+      <c r="C121" s="9">
+        <v>15.3</v>
+      </c>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
@@ -51296,6 +51668,9 @@
       <c r="B122" s="5">
         <v>7.93</v>
       </c>
+      <c r="C122" s="9">
+        <v>14.8</v>
+      </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
@@ -51304,6 +51679,9 @@
       <c r="B123" s="5">
         <v>7.95</v>
       </c>
+      <c r="C123" s="9">
+        <v>14.4</v>
+      </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
@@ -51312,6 +51690,9 @@
       <c r="B124" s="5">
         <v>7.67</v>
       </c>
+      <c r="C124" s="9">
+        <v>16.399999999999999</v>
+      </c>
       <c r="D124"/>
       <c r="O124" s="3"/>
     </row>
@@ -51322,6 +51703,9 @@
       <c r="B125" s="5">
         <v>7.72</v>
       </c>
+      <c r="C125" s="9">
+        <v>16.2</v>
+      </c>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
@@ -51330,6 +51714,9 @@
       <c r="B126" s="5">
         <v>7.77</v>
       </c>
+      <c r="C126" s="9">
+        <v>16.2</v>
+      </c>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
@@ -51338,6 +51725,9 @@
       <c r="B127" s="5">
         <v>7.8</v>
       </c>
+      <c r="C127" s="9">
+        <v>16.5</v>
+      </c>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
@@ -51346,173 +51736,239 @@
       <c r="B128" s="5">
         <v>7.89</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C128" s="9">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>175</v>
       </c>
       <c r="B129" s="5">
         <v>7.93</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C129" s="9">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>176</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C130" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>177</v>
       </c>
       <c r="B131" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C131" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>178</v>
       </c>
       <c r="B132" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C132" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>179</v>
       </c>
       <c r="B133" s="5">
         <v>7.63</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C133" s="9">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>180</v>
       </c>
       <c r="B134" s="5">
         <v>7.68</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C134" s="9">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>181</v>
       </c>
       <c r="B135" s="5">
         <v>7.76</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C135" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>182</v>
       </c>
       <c r="B136" s="5">
         <v>7.83</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C136" s="9">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>183</v>
       </c>
       <c r="B137" s="5">
         <v>7.88</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C137" s="9">
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>184</v>
       </c>
       <c r="B138" s="5">
         <v>7.94</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C138" s="9">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>185</v>
       </c>
       <c r="B139" s="5">
         <v>7.86</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C139" s="9">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>186</v>
       </c>
       <c r="B140" s="5">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C140" s="9">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>187</v>
       </c>
       <c r="B141" s="5">
         <v>7.95</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C141" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>188</v>
       </c>
       <c r="B142" s="5">
         <v>7.85</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C142" s="9">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B143" s="5">
         <v>7.88</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C143" s="9">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>190</v>
       </c>
       <c r="B144" s="5">
         <v>7.82</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C144" s="9">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>191</v>
       </c>
       <c r="B145" s="5">
         <v>7.87</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C145" s="9">
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>192</v>
       </c>
       <c r="B146" s="5">
         <v>7.97</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C146" s="9">
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>193</v>
       </c>
       <c r="B147" s="5">
         <v>7.98</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C147" s="9">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>194</v>
       </c>
       <c r="B148" s="5">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C148" s="9">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>195</v>
       </c>
       <c r="B149" s="5">
         <v>7.97</v>
+      </c>
+      <c r="C149" s="9">
+        <v>16.399999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Redone 03 to use the real temperature. Added temp to pH file recalculated the differences
</commit_message>
<xml_diff>
--- a/wk22_pH.xlsx
+++ b/wk22_pH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwdec\Documents\pH-Conversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1819F67-F627-4FFE-9BEE-28AE91E2B916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022D1432-175B-4F8C-A675-96B29A0D3E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="182">
   <si>
     <t>Sample identification number</t>
   </si>
@@ -262,24 +262,6 @@
     <t>WK22-14</t>
   </si>
   <si>
-    <t>WK22-15</t>
-  </si>
-  <si>
-    <t>WK22-16</t>
-  </si>
-  <si>
-    <t>WK22-17</t>
-  </si>
-  <si>
-    <t>WK22-18</t>
-  </si>
-  <si>
-    <t>WK22-19</t>
-  </si>
-  <si>
-    <t>WK22-20</t>
-  </si>
-  <si>
     <t>pH of sample</t>
   </si>
   <si>
@@ -487,27 +469,6 @@
     <t>WK22-84</t>
   </si>
   <si>
-    <t>WK22-85</t>
-  </si>
-  <si>
-    <t>WK22-86</t>
-  </si>
-  <si>
-    <t>WK22-87</t>
-  </si>
-  <si>
-    <t>WK22-88</t>
-  </si>
-  <si>
-    <t>WK22-89</t>
-  </si>
-  <si>
-    <t>WK22-90</t>
-  </si>
-  <si>
-    <t>WK22-91</t>
-  </si>
-  <si>
     <t>WK22-92</t>
   </si>
   <si>
@@ -568,15 +529,6 @@
     <t>WK22-111</t>
   </si>
   <si>
-    <t>WK22-112</t>
-  </si>
-  <si>
-    <t>WK22-113</t>
-  </si>
-  <si>
-    <t>WK22-114</t>
-  </si>
-  <si>
     <t>WK22-115</t>
   </si>
   <si>
@@ -628,16 +580,10 @@
     <t>WK22-132</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>pH_f</t>
   </si>
   <si>
     <t>temp_c</t>
-  </si>
-  <si>
-    <t>15,7</t>
   </si>
 </sst>
 </file>
@@ -1173,18 +1119,18 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1248,7 +1194,7 @@
         <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -50273,13 +50219,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O149"/>
+  <dimension ref="A1:O116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33:C38"/>
+      <selection pane="bottomRight" activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50295,10 +50241,10 @@
         <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -50313,1668 +50259,1299 @@
       <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>196</v>
+      <c r="A2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="5">
+        <v>7.81</v>
+      </c>
+      <c r="C2" s="9">
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>196</v>
+      <c r="A3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="5">
+        <v>7.88</v>
+      </c>
+      <c r="C3" s="9">
+        <v>15.6</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>196</v>
+      <c r="A4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="5">
+        <v>7.77</v>
+      </c>
+      <c r="C4" s="9">
+        <v>16.600000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>196</v>
+      <c r="A5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="5">
+        <v>7.93</v>
+      </c>
+      <c r="C5" s="9">
+        <v>14.1</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>196</v>
+      <c r="A6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="5">
+        <v>7.94</v>
+      </c>
+      <c r="C6" s="9">
+        <v>13.7</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>196</v>
+      <c r="A7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="5">
+        <v>7.72</v>
+      </c>
+      <c r="C7" s="9">
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>196</v>
+      <c r="A8" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="5">
+        <v>7.84</v>
+      </c>
+      <c r="C8" s="9">
+        <v>14.6</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>196</v>
+        <v>66</v>
+      </c>
+      <c r="B9" s="5">
+        <v>7.8</v>
+      </c>
+      <c r="C9" s="9">
+        <v>15.7</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>196</v>
+        <v>67</v>
+      </c>
+      <c r="B10" s="5">
+        <v>7.89</v>
+      </c>
+      <c r="C10" s="9">
+        <v>12.9</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>196</v>
+        <v>68</v>
+      </c>
+      <c r="B11" s="5">
+        <v>7.81</v>
+      </c>
+      <c r="C11" s="9">
+        <v>14.5</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>196</v>
+        <v>70</v>
+      </c>
+      <c r="B12" s="5">
+        <v>7.87</v>
+      </c>
+      <c r="C12" s="9">
+        <v>15.2</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="B13" s="5">
+        <v>7.88</v>
+      </c>
+      <c r="C13" s="9">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>196</v>
+        <v>72</v>
+      </c>
+      <c r="B14" s="5">
+        <v>7.87</v>
+      </c>
+      <c r="C14" s="9">
+        <v>15.8</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>196</v>
+        <v>73</v>
+      </c>
+      <c r="B15" s="5">
+        <v>7.87</v>
+      </c>
+      <c r="C15" s="9">
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>196</v>
+        <v>77</v>
+      </c>
+      <c r="B16" s="5">
+        <v>7.77</v>
+      </c>
+      <c r="C16" s="9">
+        <v>16.100000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>196</v>
+        <v>78</v>
+      </c>
+      <c r="B17" s="5">
+        <v>7.78</v>
+      </c>
+      <c r="C17" s="9">
+        <v>15.4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>196</v>
+        <v>79</v>
+      </c>
+      <c r="B18" s="5">
+        <v>7.85</v>
+      </c>
+      <c r="C18" s="9">
+        <v>14.6</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="B19" s="5">
-        <v>7.81</v>
+        <v>7.97</v>
       </c>
       <c r="C19" s="9">
-        <v>18.100000000000001</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="B20" s="5">
-        <v>7.88</v>
+        <v>7.78</v>
       </c>
       <c r="C20" s="9">
-        <v>15.6</v>
+        <v>14.8</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="B21" s="5">
-        <v>7.77</v>
+        <v>7.81</v>
       </c>
       <c r="C21" s="9">
-        <v>16.600000000000001</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="B22" s="5">
-        <v>7.93</v>
+        <v>7.87</v>
       </c>
       <c r="C22" s="9">
-        <v>14.1</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="B23" s="5">
-        <v>7.94</v>
+        <v>7.88</v>
       </c>
       <c r="C23" s="9">
-        <v>13.7</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="B24" s="5">
-        <v>7.72</v>
+        <v>7.93</v>
       </c>
       <c r="C24" s="9">
-        <v>16.399999999999999</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="B25" s="5">
-        <v>7.84</v>
+        <v>7.85</v>
       </c>
       <c r="C25" s="9">
-        <v>14.6</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="B26" s="5">
-        <v>7.8</v>
+        <v>7.88</v>
       </c>
       <c r="C26" s="9">
-        <v>15.7</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="B27" s="5">
-        <v>7.89</v>
+        <v>7.9</v>
       </c>
       <c r="C27" s="9">
-        <v>12.9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="B28" s="5">
-        <v>7.81</v>
+        <v>7.85</v>
       </c>
       <c r="C28" s="9">
-        <v>14.5</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="B29" s="5">
-        <v>7.87</v>
+        <v>7.81</v>
       </c>
       <c r="C29" s="9">
-        <v>15.2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="B30" s="5">
-        <v>7.88</v>
+        <v>7.79</v>
       </c>
       <c r="C30" s="9">
-        <v>15.1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="B31" s="5">
-        <v>7.87</v>
+        <v>7.78</v>
       </c>
       <c r="C31" s="9">
-        <v>15.8</v>
+        <v>14.9</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>73</v>
+      <c r="A32" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="B32" s="5">
-        <v>7.87</v>
+        <v>7.74</v>
       </c>
       <c r="C32" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>83</v>
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="5">
+        <v>7.81</v>
+      </c>
+      <c r="C33" s="9">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="5">
+        <v>7.74</v>
+      </c>
+      <c r="C34" s="9">
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="5">
+        <v>7.85</v>
+      </c>
+      <c r="C35" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="C36" s="9">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="C37" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="C38" s="9">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="B39" s="5">
-        <v>7.77</v>
+        <v>7.84</v>
       </c>
       <c r="C39" s="9">
-        <v>16.100000000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>84</v>
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="B40" s="5">
-        <v>7.78</v>
+        <v>7.8</v>
       </c>
       <c r="C40" s="9">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41" s="5">
+        <v>7.72</v>
+      </c>
+      <c r="C41" s="9">
         <v>15.4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" s="5">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B42" s="5">
+        <v>7.81</v>
+      </c>
+      <c r="C42" s="9">
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="C43" s="9">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B44" s="5">
+        <v>7.84</v>
+      </c>
+      <c r="C44" s="9">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" s="5">
         <v>7.85</v>
       </c>
-      <c r="C41" s="9">
-        <v>14.6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B42" s="5">
-        <v>7.97</v>
-      </c>
-      <c r="C42" s="9">
-        <v>15.1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B43" s="5">
-        <v>7.78</v>
-      </c>
-      <c r="C43" s="9">
-        <v>14.8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" s="5">
-        <v>7.81</v>
-      </c>
-      <c r="C44" s="9">
+      <c r="C45" s="9">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B46" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="C46" s="9">
         <v>15.5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B45" s="5">
-        <v>7.87</v>
-      </c>
-      <c r="C45" s="9">
-        <v>16.3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" s="5">
-        <v>7.88</v>
-      </c>
-      <c r="C46" s="9">
-        <v>15.8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>91</v>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="B47" s="5">
-        <v>7.93</v>
+        <v>7.83</v>
       </c>
       <c r="C47" s="9">
-        <v>14.2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>92</v>
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="B48" s="5">
-        <v>7.85</v>
+        <v>7.83</v>
       </c>
       <c r="C48" s="9">
-        <v>14.4</v>
+        <v>17.600000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>93</v>
+      <c r="A49" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="B49" s="5">
-        <v>7.88</v>
+        <v>7.15</v>
       </c>
       <c r="C49" s="9">
-        <v>13.7</v>
+        <v>18.399999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>94</v>
+      <c r="A50" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="B50" s="5">
         <v>7.9</v>
       </c>
       <c r="C50" s="9">
-        <v>14</v>
+        <v>17.3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>97</v>
+      <c r="A51" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="B51" s="5">
+        <v>7.88</v>
+      </c>
+      <c r="C51" s="9">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" s="5">
+        <v>7.86</v>
+      </c>
+      <c r="C52" s="9">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="5">
         <v>7.85</v>
       </c>
-      <c r="C51" s="9">
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B52" s="5">
-        <v>7.81</v>
-      </c>
-      <c r="C52" s="9">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B53" s="5">
-        <v>7.79</v>
-      </c>
       <c r="C53" s="9">
-        <v>14.5</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>100</v>
+      <c r="A54" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="B54" s="5">
-        <v>7.78</v>
+        <v>7.82</v>
       </c>
       <c r="C54" s="9">
-        <v>14.9</v>
+        <v>18.2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="B55" s="5">
-        <v>7.74</v>
+        <v>7.93</v>
       </c>
       <c r="C55" s="9">
-        <v>18.899999999999999</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="B56" s="5">
-        <v>7.81</v>
+        <v>7.96</v>
       </c>
       <c r="C56" s="9">
-        <v>18.5</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="B57" s="5">
-        <v>7.74</v>
+        <v>7.95</v>
       </c>
       <c r="C57" s="9">
-        <v>18.8</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="B58" s="5">
-        <v>7.85</v>
+        <v>7.94</v>
       </c>
       <c r="C58" s="9">
-        <v>19</v>
+        <v>15.3</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="B59" s="5">
-        <v>7.83</v>
+        <v>7.89</v>
       </c>
       <c r="C59" s="9">
-        <v>15.7</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="B60" s="5">
-        <v>7.83</v>
+        <v>7.92</v>
       </c>
       <c r="C60" s="9">
-        <v>16</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="B61" s="5">
-        <v>7.83</v>
+        <v>7.91</v>
       </c>
       <c r="C61" s="9">
-        <v>16.399999999999999</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="B62" s="5">
-        <v>7.84</v>
+        <v>7.94</v>
       </c>
       <c r="C62" s="9">
-        <v>15.7</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="B63" s="5">
-        <v>7.8</v>
+        <v>7.91</v>
       </c>
       <c r="C63" s="9">
-        <v>16.5</v>
+        <v>14.7</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="B64" s="5">
-        <v>7.72</v>
+        <v>7.93</v>
       </c>
       <c r="C64" s="9">
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="B65" s="5">
+        <v>7.91</v>
+      </c>
+      <c r="C65" s="9">
+        <v>14.8</v>
+      </c>
+      <c r="D65"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" s="5">
+        <v>7.94</v>
+      </c>
+      <c r="C66" s="9">
+        <v>15</v>
+      </c>
+      <c r="D66"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B67" s="5">
         <v>7.81</v>
       </c>
-      <c r="C65" s="9">
-        <v>14.3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B66" s="5">
+      <c r="C67" s="9">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="D67"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B68" s="5">
+        <v>7.68</v>
+      </c>
+      <c r="C68" s="9">
+        <v>18.7</v>
+      </c>
+      <c r="D68"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B69" s="5">
+        <v>7.81</v>
+      </c>
+      <c r="C69" s="9">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="D69"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70" s="5">
+        <v>7.84</v>
+      </c>
+      <c r="C70" s="9">
+        <v>16.7</v>
+      </c>
+      <c r="D70"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B71" s="5">
+        <v>7.94</v>
+      </c>
+      <c r="C71" s="9">
+        <v>15.3</v>
+      </c>
+      <c r="D71"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B72" s="5">
         <v>7.83</v>
       </c>
-      <c r="C66" s="9">
-        <v>14.6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B67" s="5">
-        <v>7.84</v>
-      </c>
-      <c r="C67" s="9">
-        <v>13.7</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B68" s="5">
-        <v>7.85</v>
-      </c>
-      <c r="C68" s="9">
-        <v>14.2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B69" s="5">
-        <v>7.83</v>
-      </c>
-      <c r="C69" s="9">
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B70" s="5">
-        <v>7.83</v>
-      </c>
-      <c r="C70" s="9">
-        <v>18.7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B71" s="5">
-        <v>7.83</v>
-      </c>
-      <c r="C71" s="9">
-        <v>17.600000000000001</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B72" s="5">
-        <v>7.15</v>
-      </c>
       <c r="C72" s="9">
-        <v>18.399999999999999</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="D72"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="B73" s="5">
-        <v>7.9</v>
+        <v>7.82</v>
       </c>
       <c r="C73" s="9">
-        <v>17.3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="D73"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="B74" s="5">
-        <v>7.88</v>
+        <v>8.01</v>
       </c>
       <c r="C74" s="9">
-        <v>17.100000000000001</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D74"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="B75" s="5">
-        <v>7.86</v>
+        <v>7.8</v>
       </c>
       <c r="C75" s="9">
-        <v>17.2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="D75"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="B76" s="5">
         <v>7.85</v>
       </c>
       <c r="C76" s="9">
-        <v>17.100000000000001</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20.8</v>
+      </c>
+      <c r="D76"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="B77" s="5">
+        <v>7.86</v>
+      </c>
+      <c r="C77" s="9">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D77"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78" s="5">
+        <v>7.86</v>
+      </c>
+      <c r="C78" s="9">
+        <v>18.5</v>
+      </c>
+      <c r="D78"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B79" s="5">
+        <v>7.92</v>
+      </c>
+      <c r="C79" s="9">
+        <v>15.7</v>
+      </c>
+      <c r="D79"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B80" s="5">
+        <v>7.85</v>
+      </c>
+      <c r="C80" s="9">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="D80"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B81" s="5">
+        <v>7.81</v>
+      </c>
+      <c r="C81" s="9">
+        <v>18.7</v>
+      </c>
+      <c r="D81"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B82" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="C82" s="9">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="D82"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B83" s="5">
+        <v>7.85</v>
+      </c>
+      <c r="C83" s="9">
+        <v>19.2</v>
+      </c>
+      <c r="D83"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B84" s="5">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="C84" s="9">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="D84"/>
+      <c r="O84" s="3"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B85" s="5">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="C85" s="9">
+        <v>19</v>
+      </c>
+      <c r="D85"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B86" s="5">
+        <v>7.85</v>
+      </c>
+      <c r="C86" s="9">
+        <v>18.8</v>
+      </c>
+      <c r="D86"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B87" s="5">
+        <v>7.92</v>
+      </c>
+      <c r="C87" s="9">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B88" s="5">
+        <v>7.76</v>
+      </c>
+      <c r="C88" s="9">
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B89" s="5">
+        <v>7.81</v>
+      </c>
+      <c r="C89" s="9">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B90" s="5">
         <v>7.82</v>
       </c>
-      <c r="C77" s="9">
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B78" s="5">
+      <c r="C90" s="9">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B91" s="5">
+        <v>7.89</v>
+      </c>
+      <c r="C91" s="9">
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B92" s="5">
         <v>7.93</v>
       </c>
-      <c r="C78" s="9">
+      <c r="C92" s="9">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B93" s="5">
+        <v>7.95</v>
+      </c>
+      <c r="C93" s="9">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B94" s="5">
+        <v>7.67</v>
+      </c>
+      <c r="C94" s="9">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="D94"/>
+      <c r="O94" s="3"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B95" s="5">
+        <v>7.72</v>
+      </c>
+      <c r="C95" s="9">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B96" s="5">
+        <v>7.77</v>
+      </c>
+      <c r="C96" s="9">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B97" s="5">
+        <v>7.8</v>
+      </c>
+      <c r="C97" s="9">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B98" s="5">
+        <v>7.89</v>
+      </c>
+      <c r="C98" s="9">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B99" s="5">
+        <v>7.93</v>
+      </c>
+      <c r="C99" s="9">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B100" s="5">
+        <v>7.63</v>
+      </c>
+      <c r="C100" s="9">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B101" s="5">
+        <v>7.68</v>
+      </c>
+      <c r="C101" s="9">
         <v>15.4</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B79" s="5">
-        <v>7.96</v>
-      </c>
-      <c r="C79" s="9">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B102" s="5">
+        <v>7.76</v>
+      </c>
+      <c r="C102" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B103" s="5">
+        <v>7.83</v>
+      </c>
+      <c r="C103" s="9">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B104" s="5">
+        <v>7.88</v>
+      </c>
+      <c r="C104" s="9">
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B105" s="5">
+        <v>7.94</v>
+      </c>
+      <c r="C105" s="9">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B106" s="5">
+        <v>7.86</v>
+      </c>
+      <c r="C106" s="9">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B107" s="5">
+        <v>7.9</v>
+      </c>
+      <c r="C107" s="9">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B108" s="5">
+        <v>7.95</v>
+      </c>
+      <c r="C108" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B109" s="5">
+        <v>7.85</v>
+      </c>
+      <c r="C109" s="9">
         <v>15.4</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B80" s="5">
-        <v>7.95</v>
-      </c>
-      <c r="C80" s="9">
-        <v>15.2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B81" s="5">
-        <v>7.94</v>
-      </c>
-      <c r="C81" s="9">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B110" s="5">
+        <v>7.88</v>
+      </c>
+      <c r="C110" s="9">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B111" s="5">
+        <v>7.82</v>
+      </c>
+      <c r="C111" s="9">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B112" s="5">
+        <v>7.87</v>
+      </c>
+      <c r="C112" s="9">
         <v>15.3</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B82" s="5">
-        <v>7.89</v>
-      </c>
-      <c r="C82" s="9">
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B83" s="5">
-        <v>7.92</v>
-      </c>
-      <c r="C83" s="9">
-        <v>15.8</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B84" s="5">
-        <v>7.91</v>
-      </c>
-      <c r="C84" s="9">
-        <v>15.1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B85" s="5">
-        <v>7.94</v>
-      </c>
-      <c r="C85" s="9">
-        <v>14.1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B86" s="5">
-        <v>7.91</v>
-      </c>
-      <c r="C86" s="9">
-        <v>14.7</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B87" s="5">
-        <v>7.93</v>
-      </c>
-      <c r="C87" s="9">
-        <v>14.9</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B88" s="5">
-        <v>7.91</v>
-      </c>
-      <c r="C88" s="9">
-        <v>14.8</v>
-      </c>
-      <c r="D88"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B89" s="5">
-        <v>7.94</v>
-      </c>
-      <c r="C89" s="9">
-        <v>15</v>
-      </c>
-      <c r="D89"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B90" s="5">
-        <v>7.81</v>
-      </c>
-      <c r="C90" s="9">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="D90"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B91" s="5">
-        <v>7.68</v>
-      </c>
-      <c r="C91" s="9">
-        <v>18.7</v>
-      </c>
-      <c r="D91"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B92" s="5">
-        <v>7.81</v>
-      </c>
-      <c r="C92" s="9">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="D92"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B93" s="5">
-        <v>7.84</v>
-      </c>
-      <c r="C93" s="9">
-        <v>16.7</v>
-      </c>
-      <c r="D93"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B94" s="5">
-        <v>7.94</v>
-      </c>
-      <c r="C94" s="9">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B113" s="5">
+        <v>7.97</v>
+      </c>
+      <c r="C113" s="9">
         <v>15.3</v>
       </c>
-      <c r="D94"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B95" s="5">
-        <v>7.83</v>
-      </c>
-      <c r="C95" s="9">
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B114" s="5">
+        <v>7.98</v>
+      </c>
+      <c r="C114" s="9">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B115" s="5">
+        <v>7.9</v>
+      </c>
+      <c r="C115" s="9">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B116" s="5">
+        <v>7.97</v>
+      </c>
+      <c r="C116" s="9">
         <v>16.399999999999999</v>
       </c>
-      <c r="D95"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B96" s="5">
-        <v>7.82</v>
-      </c>
-      <c r="C96" s="9">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="D96"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B97" s="5">
-        <v>8.01</v>
-      </c>
-      <c r="C97" s="9">
-        <v>18</v>
-      </c>
-      <c r="D97"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B98" s="5">
-        <v>7.8</v>
-      </c>
-      <c r="C98" s="9">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="D98"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B99" s="5">
-        <v>7.85</v>
-      </c>
-      <c r="C99" s="9">
-        <v>20.8</v>
-      </c>
-      <c r="D99"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B100" s="5">
-        <v>7.86</v>
-      </c>
-      <c r="C100" s="9">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="D100"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B101" s="5">
-        <v>7.86</v>
-      </c>
-      <c r="C101" s="9">
-        <v>18.5</v>
-      </c>
-      <c r="D101"/>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B102" s="5">
-        <v>7.92</v>
-      </c>
-      <c r="C102" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="D102"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C103" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D103"/>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C104" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D104"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C105" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D105"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C106" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D106"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B107" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C107" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D107"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C108" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D108"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C109" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D109"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B110" s="5">
-        <v>7.85</v>
-      </c>
-      <c r="C110" s="9">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="D110"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B111" s="5">
-        <v>7.81</v>
-      </c>
-      <c r="C111" s="9">
-        <v>18.7</v>
-      </c>
-      <c r="D111"/>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B112" s="5">
-        <v>7.83</v>
-      </c>
-      <c r="C112" s="9">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="D112"/>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B113" s="5">
-        <v>7.85</v>
-      </c>
-      <c r="C113" s="9">
-        <v>19.2</v>
-      </c>
-      <c r="D113"/>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B114" s="5">
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="C114" s="9">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="D114"/>
-      <c r="O114" s="3"/>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B115" s="5">
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="C115" s="9">
-        <v>19</v>
-      </c>
-      <c r="D115"/>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B116" s="5">
-        <v>7.85</v>
-      </c>
-      <c r="C116" s="9">
-        <v>18.8</v>
-      </c>
-      <c r="D116"/>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B117" s="5">
-        <v>7.92</v>
-      </c>
-      <c r="C117" s="9">
-        <v>18.899999999999999</v>
-      </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B118" s="5">
-        <v>7.76</v>
-      </c>
-      <c r="C118" s="9">
-        <v>15.3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B119" s="5">
-        <v>7.81</v>
-      </c>
-      <c r="C119" s="9"/>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B120" s="5">
-        <v>7.82</v>
-      </c>
-      <c r="C120" s="9">
-        <v>15.2</v>
-      </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B121" s="5">
-        <v>7.89</v>
-      </c>
-      <c r="C121" s="9">
-        <v>15.3</v>
-      </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A122" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B122" s="5">
-        <v>7.93</v>
-      </c>
-      <c r="C122" s="9">
-        <v>14.8</v>
-      </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A123" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B123" s="5">
-        <v>7.95</v>
-      </c>
-      <c r="C123" s="9">
-        <v>14.4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A124" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B124" s="5">
-        <v>7.67</v>
-      </c>
-      <c r="C124" s="9">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="D124"/>
-      <c r="O124" s="3"/>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A125" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B125" s="5">
-        <v>7.72</v>
-      </c>
-      <c r="C125" s="9">
-        <v>16.2</v>
-      </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A126" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B126" s="5">
-        <v>7.77</v>
-      </c>
-      <c r="C126" s="9">
-        <v>16.2</v>
-      </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A127" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B127" s="5">
-        <v>7.8</v>
-      </c>
-      <c r="C127" s="9">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A128" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B128" s="5">
-        <v>7.89</v>
-      </c>
-      <c r="C128" s="9">
-        <v>16.3</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B129" s="5">
-        <v>7.93</v>
-      </c>
-      <c r="C129" s="9">
-        <v>16.399999999999999</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B130" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C130" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B131" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C131" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B132" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C132" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B133" s="5">
-        <v>7.63</v>
-      </c>
-      <c r="C133" s="9">
-        <v>15.1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B134" s="5">
-        <v>7.68</v>
-      </c>
-      <c r="C134" s="9">
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B135" s="5">
-        <v>7.76</v>
-      </c>
-      <c r="C135" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B136" s="5">
-        <v>7.83</v>
-      </c>
-      <c r="C136" s="9">
-        <v>14.2</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B137" s="5">
-        <v>7.88</v>
-      </c>
-      <c r="C137" s="9">
-        <v>14.3</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B138" s="5">
-        <v>7.94</v>
-      </c>
-      <c r="C138" s="9">
-        <v>14.8</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B139" s="5">
-        <v>7.86</v>
-      </c>
-      <c r="C139" s="9">
-        <v>13.4</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="B140" s="5">
-        <v>7.9</v>
-      </c>
-      <c r="C140" s="9">
-        <v>13.2</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B141" s="5">
-        <v>7.95</v>
-      </c>
-      <c r="C141" s="9">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B142" s="5">
-        <v>7.85</v>
-      </c>
-      <c r="C142" s="9">
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B143" s="5">
-        <v>7.88</v>
-      </c>
-      <c r="C143" s="9">
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B144" s="5">
-        <v>7.82</v>
-      </c>
-      <c r="C144" s="9">
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B145" s="5">
-        <v>7.87</v>
-      </c>
-      <c r="C145" s="9">
-        <v>15.3</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B146" s="5">
-        <v>7.97</v>
-      </c>
-      <c r="C146" s="9">
-        <v>15.3</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B147" s="5">
-        <v>7.98</v>
-      </c>
-      <c r="C147" s="9">
-        <v>13.7</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B148" s="5">
-        <v>7.9</v>
-      </c>
-      <c r="C148" s="9">
-        <v>17.2</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B149" s="5">
-        <v>7.97</v>
-      </c>
-      <c r="C149" s="9">
-        <v>16.399999999999999</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D89:N115">
-    <sortCondition ref="D89:D115"/>
-    <sortCondition ref="N89:N115"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D66:N85">
+    <sortCondition ref="D66:D85"/>
+    <sortCondition ref="N66:N85"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>